<commit_message>
Circulation Course - ajout et fin
- Fin de la page circulation en course
- Traduction en anglais
- Ajout des images tirées du guide d'organisation UCI
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3984AAF3-38BA-2949-9761-64590E2A5384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266FB7CC-1A6A-F641-B032-B3859F236929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="560" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="60" yWindow="560" windowWidth="33480" windowHeight="20380" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -316,9 +316,6 @@
     <t>Vincent Drouin&lt;br/&gt;Justine Boucher</t>
   </si>
   <si>
-    <t xml:space="preserve">Présidente du Collège des commissaires </t>
-  </si>
-  <si>
     <t xml:space="preserve">President of the Commissaires Panel </t>
   </si>
   <si>
@@ -326,9 +323,6 @@
   </si>
   <si>
     <t>role_fr</t>
-  </si>
-  <si>
-    <t>Thierry D</t>
   </si>
   <si>
     <t>Commissaires</t>
@@ -427,6 +421,12 @@
   </si>
   <si>
     <t>Technical director</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Président du Collège des commissaires </t>
+  </si>
+  <si>
+    <t>Thierry Diederen</t>
   </si>
 </sst>
 </file>
@@ -852,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -866,10 +866,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -880,16 +880,16 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -903,12 +903,12 @@
         <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -917,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -931,7 +931,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -945,7 +945,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -959,7 +959,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -987,7 +987,7 @@
         <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1001,7 +1001,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1043,7 +1043,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1057,7 +1057,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1071,7 +1071,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1085,7 +1085,7 @@
         <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1099,7 +1099,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1113,7 +1113,7 @@
         <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1127,7 +1127,7 @@
         <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1141,7 +1141,7 @@
         <v>61</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1155,7 +1155,7 @@
         <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1169,7 +1169,7 @@
         <v>49</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1183,7 +1183,7 @@
         <v>50</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1209,10 +1209,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -1251,7 +1251,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>77</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>78</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>84</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1364,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823BAD0D-314A-CF4D-A7B3-D837A1000984}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1377,10 +1377,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -1388,35 +1388,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modif noms de Staff
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC995A0-01AC-A64D-A459-A49D47BADF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A942B21-0413-7147-89EC-03627A45140A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16480" yWindow="3720" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="120" yWindow="620" windowWidth="33480" windowHeight="20380" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t xml:space="preserve">Suzanne Fortin </t>
   </si>
   <si>
-    <t>Isabelle Gosselin</t>
-  </si>
-  <si>
     <t>Coordonator - Tour Abitibi</t>
   </si>
   <si>
@@ -319,102 +316,105 @@
     <t>Marc Dufour&lt;br/&gt;Centrifuge</t>
   </si>
   <si>
+    <t>Présidente du CA</t>
+  </si>
+  <si>
+    <t>\(819) 527-7623</t>
+  </si>
+  <si>
+    <t>\(819) 290-3612</t>
+  </si>
+  <si>
+    <t>\(819) 290-8834</t>
+  </si>
+  <si>
+    <t>\(819) 355-1740</t>
+  </si>
+  <si>
+    <t>\(819) 444-6975</t>
+  </si>
+  <si>
+    <t>\(819) 732-4038</t>
+  </si>
+  <si>
+    <t>\(819) 732-0094</t>
+  </si>
+  <si>
+    <t>\(819) 444-8887&lt;br/&gt;(418) 690-6564</t>
+  </si>
+  <si>
+    <t>\(819) 444-9746</t>
+  </si>
+  <si>
+    <t>\(819) 277-1889</t>
+  </si>
+  <si>
+    <t>\(819) 856-6040</t>
+  </si>
+  <si>
+    <t>\(819) 444-6221&lt;br/&gt;(819) 734-7105</t>
+  </si>
+  <si>
+    <t>\(819) 443-2386&lt;br/&gt;(819) 444-8518</t>
+  </si>
+  <si>
+    <t>\(819) 444-6389&lt;br/&gt;(819) 856-4608</t>
+  </si>
+  <si>
+    <t>\(819) 442-3505</t>
+  </si>
+  <si>
+    <t>\(819) 856-1803</t>
+  </si>
+  <si>
+    <t>Roxanne Pépin, Dt.P.</t>
+  </si>
+  <si>
+    <t>Chairwoman of the board</t>
+  </si>
+  <si>
+    <t>Technical director</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Président du Collège des commissaires </t>
+  </si>
+  <si>
+    <t>David Bernard</t>
+  </si>
+  <si>
+    <t>Project manager - Tour de l’Abitibi</t>
+  </si>
+  <si>
+    <t>Project manager - Tour de la Relève</t>
+  </si>
+  <si>
+    <t>Christine Beausoleil&lt;br/&gt;Pierrick Naud</t>
+  </si>
+  <si>
+    <t>\(819) 355-3202&lt;br/&gt;(514) 647-6659</t>
+  </si>
+  <si>
+    <t>\(819) 555-1212</t>
+  </si>
+  <si>
+    <t>Thierry Diederen&lt;br/&gt;thierry.diederen@hotmail.be</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Ville d'Amos</t>
+  </si>
+  <si>
+    <t>Myriam Audet</t>
+  </si>
+  <si>
     <t>Louise Lalonde&lt;br/&gt;
-Johanne Binet&lt;br/&gt;
+Michel Bourgault&lt;br/&gt;
 Hélène Soulard&lt;br/&gt;
 Valérie Trottier&lt;br/&gt;
 Nancy Daigle&lt;br/&gt;
 Simon Bouchard</t>
-  </si>
-  <si>
-    <t>Présidente du CA</t>
-  </si>
-  <si>
-    <t>\(819) 527-7623</t>
-  </si>
-  <si>
-    <t>\(819) 290-3612</t>
-  </si>
-  <si>
-    <t>\(819) 290-8834</t>
-  </si>
-  <si>
-    <t>\(819) 355-1740</t>
-  </si>
-  <si>
-    <t>\(819) 444-6975</t>
-  </si>
-  <si>
-    <t>\(819) 732-4038</t>
-  </si>
-  <si>
-    <t>\(819) 732-0094</t>
-  </si>
-  <si>
-    <t>\(819) 444-8887&lt;br/&gt;(418) 690-6564</t>
-  </si>
-  <si>
-    <t>\(819) 444-9746</t>
-  </si>
-  <si>
-    <t>\(819) 277-1889</t>
-  </si>
-  <si>
-    <t>\(819) 856-6040</t>
-  </si>
-  <si>
-    <t>\(819) 444-6221&lt;br/&gt;(819) 734-7105</t>
-  </si>
-  <si>
-    <t>\(819) 443-2386&lt;br/&gt;(819) 444-8518</t>
-  </si>
-  <si>
-    <t>\(819) 444-6389&lt;br/&gt;(819) 856-4608</t>
-  </si>
-  <si>
-    <t>\(819) 442-3505</t>
-  </si>
-  <si>
-    <t>\(819) 856-1803</t>
-  </si>
-  <si>
-    <t>Roxanne Pépin, Dt.P.</t>
-  </si>
-  <si>
-    <t>Chairwoman of the board</t>
-  </si>
-  <si>
-    <t>Technical director</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Président du Collège des commissaires </t>
-  </si>
-  <si>
-    <t>David Bernard</t>
-  </si>
-  <si>
-    <t>Project manager - Tour de l’Abitibi</t>
-  </si>
-  <si>
-    <t>Project manager - Tour de la Relève</t>
-  </si>
-  <si>
-    <t>Christine Beausoleil&lt;br/&gt;Pierrick Naud</t>
-  </si>
-  <si>
-    <t>\(819) 355-3202&lt;br/&gt;(514) 647-6659</t>
-  </si>
-  <si>
-    <t>\(819) 555-1212</t>
-  </si>
-  <si>
-    <t>Thierry Diederen&lt;br/&gt;thierry.diederen@hotmail.be</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Ville d'Amos</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -579,7 +579,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -685,7 +685,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -851,10 +851,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -865,35 +865,35 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -902,7 +902,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -913,38 +913,38 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -958,7 +958,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -969,10 +969,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -997,10 +997,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1011,10 +1011,10 @@
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1028,7 +1028,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1056,7 +1056,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1067,10 +1067,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,10 +1081,10 @@
         <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1095,10 +1095,10 @@
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1109,10 +1109,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1123,10 +1123,10 @@
         <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1140,7 +1140,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1151,24 +1151,24 @@
         <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1194,10 +1194,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1205,120 +1205,120 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>20</v>
@@ -1326,13 +1326,13 @@
     </row>
     <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1349,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823BAD0D-314A-CF4D-A7B3-D837A1000984}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,10 +1362,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1373,35 +1373,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" t="s">
         <v>90</v>
-      </c>
-      <c r="C4" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modif commanditaires, web et pdf
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFF2CDF-CC48-9C4D-B222-990F3B60CC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584313AC-98F0-2041-B180-CA80E57367CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="102460" yWindow="4240" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
@@ -175,9 +175,6 @@
     <t>Coordonator - Tour Abitibi</t>
   </si>
   <si>
-    <t>Étudiant</t>
-  </si>
-  <si>
     <t>Pierre Galarneau&lt;br/&gt;France Galarneau</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>Philippe Vallière&lt;br/&gt;Michaël  Bouchard</t>
+  </si>
+  <si>
+    <t>Amélie Gélinas</t>
   </si>
 </sst>
 </file>
@@ -877,7 +877,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,10 +890,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -904,16 +904,16 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -924,15 +924,15 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -952,38 +952,38 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -997,7 +997,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1008,10 +1008,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1025,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1036,10 +1036,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1047,13 +1047,13 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1067,7 +1067,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1095,7 +1095,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1106,10 +1106,10 @@
         <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1123,7 +1123,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1134,10 +1134,10 @@
         <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1148,10 +1148,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1162,10 +1162,10 @@
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1173,13 +1173,13 @@
         <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1190,24 +1190,24 @@
         <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1233,10 +1233,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1244,131 +1244,131 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>20</v>
@@ -1376,13 +1376,13 @@
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1412,10 +1412,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1423,35 +1423,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" t="s">
         <v>82</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout responsable Tour Relève au guide
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584313AC-98F0-2041-B180-CA80E57367CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81135FB1-B9CC-0D48-B50B-DD78AA6F83A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="102460" yWindow="4240" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="33380" yWindow="3380" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="134">
   <si>
     <t>noms</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Mélanie Rocher</t>
-  </si>
-  <si>
-    <t>Coordonnatrice du Tour</t>
   </si>
   <si>
     <t>Directeur technique</t>
@@ -436,6 +433,18 @@
   </si>
   <si>
     <t>Amélie Gélinas</t>
+  </si>
+  <si>
+    <t>Pascal Sayeur&lt;br/&gt;David Bernard</t>
+  </si>
+  <si>
+    <t>\(819) 444-7760 &lt;br/&gt;\(819) 734-7897</t>
+  </si>
+  <si>
+    <t>Tour de la Relève</t>
+  </si>
+  <si>
+    <t>Coordonnatrice du Tour de l'Abitibi</t>
   </si>
 </sst>
 </file>
@@ -874,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,10 +899,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -904,310 +913,324 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>95</v>
+      <c r="C24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1233,10 +1256,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1244,145 +1267,145 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1412,10 +1435,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1423,35 +1446,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout cell CP Tour
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81135FB1-B9CC-0D48-B50B-DD78AA6F83A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA3784-BE2D-1342-87B4-519D081FF60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33380" yWindow="3380" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t xml:space="preserve">Assistant technical director </t>
   </si>
   <si>
-    <t>Chargé de projet Tour de la relève</t>
-  </si>
-  <si>
     <t>Chargé de projet Tour de l’Abitibi</t>
   </si>
   <si>
@@ -420,9 +417,6 @@
     <t>\(418) 690-6564</t>
   </si>
   <si>
-    <t>\(819) 555-xxxx</t>
-  </si>
-  <si>
     <t>Ardoisière</t>
   </si>
   <si>
@@ -445,6 +439,12 @@
   </si>
   <si>
     <t>Coordonnatrice du Tour de l'Abitibi</t>
+  </si>
+  <si>
+    <t>Chargé de projet Tour de la Relève</t>
+  </si>
+  <si>
+    <t>\(819) 727-6333</t>
   </si>
 </sst>
 </file>
@@ -886,7 +886,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,10 +899,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -913,35 +913,35 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -950,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -961,276 +961,276 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1256,10 +1256,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1267,145 +1267,145 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1435,10 +1435,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1446,35 +1446,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustement staff et mot ministre
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6FDAC3-DC5F-054A-A44F-50B8BA990CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB65E573-CE2D-7947-AB69-B559E46B0E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33380" yWindow="3380" windowWidth="33480" windowHeight="20380" activeTab="1" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
@@ -235,9 +235,6 @@
     <t>Speaker</t>
   </si>
   <si>
-    <t>TBC</t>
-  </si>
-  <si>
     <t>Ambulance</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>Marco Prévost</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Bobby Noury</t>
   </si>
   <si>
@@ -445,6 +439,12 @@
   </si>
   <si>
     <t>Maurice Normand&lt;br/&gt;Chantal Gélinas</t>
+  </si>
+  <si>
+    <t>Dominic Lafleur&lt;br/&gt;Justine Boucher</t>
+  </si>
+  <si>
+    <t>Josyane Bolduc</t>
   </si>
 </sst>
 </file>
@@ -899,10 +899,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -913,16 +913,16 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -930,18 +930,18 @@
         <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -950,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -961,38 +961,38 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1006,7 +1006,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,7 +1020,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1034,7 +1034,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1048,7 +1048,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1056,13 +1056,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1076,7 +1076,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1090,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1118,7 +1118,7 @@
         <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1132,7 +1132,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1143,10 +1143,10 @@
         <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1157,10 +1157,10 @@
         <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1171,10 +1171,10 @@
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1182,13 +1182,13 @@
         <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1199,24 +1199,24 @@
         <v>39</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1230,7 +1230,7 @@
         <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1244,7 +1244,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1256,10 +1256,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1273,7 +1273,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1292,7 +1292,7 @@
         <v>58</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>49</v>
@@ -1306,7 +1306,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>62</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1339,26 +1339,26 @@
         <v>51</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>53</v>
@@ -1377,21 +1377,21 @@
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
@@ -1399,13 +1399,13 @@
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1435,10 +1435,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1446,35 +1446,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" t="s">
         <v>78</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>